<commit_message>
Started translation of req list to english
Started translation of req list to english
</commit_message>
<xml_diff>
--- a/requirements/Requirement List.xlsx
+++ b/requirements/Requirement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SS-PC\Ciorne\SistemVotElectronic\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B8F201-F464-4D14-A202-AA05D0ABC090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6FBD90-B79C-4FB1-953E-651079F4AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="129">
   <si>
     <t>Requirements Document</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Aplicatia poate fi lansata din consola</t>
-  </si>
-  <si>
-    <t>Aplicatia ramane in memorie pe un termen nedefinit, indiferent de numarul de stari prin care trece sau de timpul petrecut in aceeasi stare</t>
-  </si>
-  <si>
     <t>Requirement met ?</t>
   </si>
   <si>
@@ -67,19 +61,7 @@
     <t>R003</t>
   </si>
   <si>
-    <t>La lansare, aplicatia incarca in memorie ID-ul sectiei de votare</t>
-  </si>
-  <si>
-    <t>ver DEBUG: Incarca din fisier txt; ver RELEASE: Incarca printr-un server request</t>
-  </si>
-  <si>
     <t>R004</t>
-  </si>
-  <si>
-    <t>DEBUG Only</t>
-  </si>
-  <si>
-    <t>Aplicatia poate fi oprita din consola sau dintr-un buton dedicat de oprire fortata</t>
   </si>
   <si>
     <t>G001</t>
@@ -391,25 +373,62 @@
     <t>R050</t>
   </si>
   <si>
-    <t>Fiecare Buletin de Vot este format dintr-o clasa ce contine toate informatiile relevante pentru un Buletin de Vot</t>
-  </si>
-  <si>
-    <t>Sesiunea de Vot este formata dintr-o clasa, ce contine toate informatiile relevante pentru o Sesiune de Vot</t>
-  </si>
-  <si>
-    <t>Relatia de tip "has-a" - "one-to-many"</t>
-  </si>
-  <si>
-    <t>Sesiunea de Vot contine o lista cu unul sau mai multe Buletine de Vot</t>
-  </si>
-  <si>
-    <t>Buletinele de Vot si Sesiune de Vot sunt transmise de catre server la aplicatia client in format JSON</t>
-  </si>
-  <si>
-    <t>La lansare, aplicatia intra in prima stare in care asteapta confirmare de la cititorul NFC</t>
-  </si>
-  <si>
-    <t>Aplicatia trece in a doua stare numai dupa ce a fost citit un mesaj valid de cititorul NFC</t>
+    <t>Aplicatia poate fi lansata din consola
+The App can be launched from the console</t>
+  </si>
+  <si>
+    <t>Aplicatia ramane in memorie pe un termen nedefinit, indiferent de numarul de stari prin care trece sau de timpul petrecut in aceeasi stare
+The App remains loaded in memory undefinitely, no matter the number of states it switches or the time elapsed in any given state, until it is closed (by session end or forced to close)</t>
+  </si>
+  <si>
+    <t>Aplicatia poate fi oprita din consola sau dintr-un buton dedicat de oprire fortata
+The App can be stopped from the console (session end) or via the Force Quit button</t>
+  </si>
+  <si>
+    <t>Force Quit button for DEBUG purposes Only</t>
+  </si>
+  <si>
+    <t>La lansare, aplicatia incarca in memorie ID-ul sectiei de votare
+On launch, the App loads in the RAM all the information and the Voting Section ID</t>
+  </si>
+  <si>
+    <t>in DEBUG: load from txt FILE; in RELEASE: load via server request</t>
+  </si>
+  <si>
+    <t>La lansare, aplicatia intra in prima stare in care asteapta confirmare de la cititorul NFC
+On launch, the App enters the first state, where it awaits an NFC Reader message</t>
+  </si>
+  <si>
+    <t>Aplicatia trece in a doua stare numai dupa ce a fost citit un mesaj valid de cititorul NFC
+The App switches to the next state ONLY after the NFC Reader message is received</t>
+  </si>
+  <si>
+    <t>DEBUG mode: The NFC Reader message is emulated by using a Button in the GUI (&gt;&gt;reference to GUI Req)</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Fiecare Buletin de Vot este format dintr-o clasa ce contine toate informatiile relevante pentru un Buletin de Vot
+Each Vote Ballot is represented by a Class which contains all the relevant for a Vote Ballot</t>
+  </si>
+  <si>
+    <t>A  "has-a" - "one-to-many" relationship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buletinele de Vot si Sesiune de Vot sunt transmise de catre server la aplicatia client in format JSON
+The Vote Ballots and Vote sessions are transmitted by the Server to the Client App using the JSON format </t>
+  </si>
+  <si>
+    <t>Sesiunea de Vot contine o lista cu unul sau mai multe Buletine de Vot
+A Vote Session contains a list with one or more Vote Ballots</t>
+  </si>
+  <si>
+    <t>Sesiunea de Vot este formata dintr-o clasa, ce contine toate informatiile relevante pentru o Sesiune de Vot
+Each Vote Session is represented by a Class which contains all the relevant data for a Voting Session</t>
   </si>
 </sst>
 </file>
@@ -481,9 +500,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -503,6 +519,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,42 +802,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F6:L8"/>
+  <dimension ref="F6:W8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6:W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F6" s="1" t="s">
+    <row r="6" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="W6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="W7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -833,331 +858,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281B815F-C85E-422A-83E0-3E992CFD935E}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="126.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="126.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="B2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B19" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1179,20 +1208,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1210,296 +1239,296 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="102" style="5" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="102" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1512,34 +1541,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C4964E-64FC-4281-92CE-21988E04702A}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="130.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="130.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of requirement list
</commit_message>
<xml_diff>
--- a/requirements/Requirement List.xlsx
+++ b/requirements/Requirement List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SS-PC\Ciorne\SistemVotElectronic\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF65ECE2-5E18-46BE-B635-FFCA34E702CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095A451E-DD56-429A-AE5E-BA0D83529ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2790" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -418,35 +418,35 @@
     <t>When the App is launched, the Main Window is drawn Fullscreen</t>
   </si>
   <si>
-    <t>The App is comprised of 4 different Views: 
+    <t>The Main Window is a Welcome Screen, showing a Greeting message</t>
+  </si>
+  <si>
+    <t>also a Button for DEBUG mode, to move to next screen</t>
+  </si>
+  <si>
+    <t>The Vote Session Window shows a list of active Voting Sessions, as a List from which the USER can select one</t>
+  </si>
+  <si>
+    <t>The Vote Ballot Window shows a list of all the Candidates, as a Grid of elements spannig across multiple pages (if required), from which the USER can only select one at a time</t>
+  </si>
+  <si>
+    <t>The Exit Window shows a Farewell message and is shown only for a set time, after which the App switches back to the Main Window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the App is launched, the Quit, Minimize and Maximize are no longer visible </t>
+  </si>
+  <si>
+    <t>May be skipped</t>
+  </si>
+  <si>
+    <t>The Main Window has 3 graphical elements: a Quit Button, an image to guide the USER to where the NFC Reader is placed and a Greeting Message containing the Voting Precint ID</t>
+  </si>
+  <si>
+    <t>The App is composed of 4 different Views: 
 1. Main Window
 2. Vote Session Window
 3. Vote Ballot Window
 4. Exit Window</t>
-  </si>
-  <si>
-    <t>The Main Window is a Welcome Screen, showing a Greeting message</t>
-  </si>
-  <si>
-    <t>also a Button for DEBUG mode, to move to next screen</t>
-  </si>
-  <si>
-    <t>The Vote Session Window shows a list of active Voting Sessions, as a List from which the USER can select one</t>
-  </si>
-  <si>
-    <t>The Vote Ballot Window shows a list of all the Candidates, as a Grid of elements spannig across multiple pages (if required), from which the USER can only select one at a time</t>
-  </si>
-  <si>
-    <t>The Exit Window shows a Farewell message and is shown only for a set time, after which the App switches back to the Main Window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the App is launched, the Quit, Minimize and Maximize are no longer visible </t>
-  </si>
-  <si>
-    <t>May be skipped</t>
-  </si>
-  <si>
-    <t>The Main Window has 3 graphical elements: a Quit Button, an image to guide the USER to where the NFC Reader is placed and a Greeting Message containing the Voting Precint ID</t>
   </si>
 </sst>
 </file>
@@ -879,14 +879,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281B815F-C85E-422A-83E0-3E992CFD935E}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="126.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="49.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
@@ -923,7 +923,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -940,7 +940,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -991,7 +991,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -1332,14 +1332,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF32260F-DDFA-4B26-857F-93BFC373C56C}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="102" style="4" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
@@ -1381,10 +1381,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>112</v>
@@ -1398,10 +1398,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>112</v>
@@ -1410,12 +1410,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>112</v>
@@ -1424,12 +1424,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>112</v>
@@ -1438,12 +1438,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>112</v>
@@ -1452,12 +1452,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>112</v>
@@ -1471,7 +1471,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
@@ -1715,7 +1715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C4964E-64FC-4281-92CE-21988E04702A}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>